<commit_message>
Error handling updated - select make for car 1.
</commit_message>
<xml_diff>
--- a/cars.xlsx
+++ b/cars.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dee\Documents\UiPath\Assignment2-NotGreat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dee\Documents\UiPath\Assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57AFADD2-E59F-4B4B-A134-9A5DCC5DC6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7788FD59-9C50-45AE-B126-66023B3572A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5550" yWindow="2205" windowWidth="21600" windowHeight="7575" xr2:uid="{6F4DCAE2-0BA8-4075-A207-16147C0730BD}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{6F4DCAE2-0BA8-4075-A207-16147C0730BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="177">
   <si>
     <t>Nou
 Smart fortwo EQ 60kWed cool&amp;Audio SHZ Tempom Klima</t>
@@ -538,6 +538,72 @@
   <si>
     <t>Nou
 Smart smart EQ fortwo Cool u. Audio Einparkhilfe</t>
+  </si>
+  <si>
+    <t>Nou
+Smart fortwo EQ Bremsassi.+Tempomat+Cool&amp;Audio P.+15</t>
+  </si>
+  <si>
+    <t>Nou
+Smart SMART EQ FORTWO COOL &amp; AUDIO-PAKET</t>
+  </si>
+  <si>
+    <t>Nou
+Smart smart fortwo electric drive Tempomat Klima</t>
+  </si>
+  <si>
+    <t>Nou
+Smart fortwo EQ 60kWed passion cool&amp;Audio SHZ Komfort</t>
+  </si>
+  <si>
+    <t>Nou
+Smart EQ fortwo electric drive Cool &amp; Audio Klima</t>
+  </si>
+  <si>
+    <t>Nou
+Smart fortwo EQ 60kWed passion SHZ Pano PDC+Kamera</t>
+  </si>
+  <si>
+    <t>Nou
+Smart SMART FORTWO ELECTRIC DRIVE</t>
+  </si>
+  <si>
+    <t>Nou
+Smart EQ fortwo Passion Cool u. Audio,Sitze schwarz</t>
+  </si>
+  <si>
+    <t>Nou
+Smart Fortwo cabrio electric drive / EQ &gt;NAV/SHZ/TEMP&lt;</t>
+  </si>
+  <si>
+    <t>Nou
+Smart ForTwo Coupe EQ Prime 22kw 1. Hand HU 5/24 MwSt</t>
+  </si>
+  <si>
+    <t>Nou
+Smart fortwo coupe electric drive / EQ *Erst 2900KM*</t>
+  </si>
+  <si>
+    <t>Nou
+Smart fortwo + SPORTFAKET + NEBELSCHEINWERFER+ KLIMAAU</t>
+  </si>
+  <si>
+    <t>Smart smart fortwo cabrio electric drive</t>
+  </si>
+  <si>
+    <t>Smart smart EQ fortwo 22KW Lader Cool Media Pano Sitzh</t>
+  </si>
+  <si>
+    <t>Smart Fortwo Coupe Electric Drive / EQ*Navi*RFk*Klima*</t>
+  </si>
+  <si>
+    <t>Smart ForTwo coupé I Passion I Panorama I Touch I SHZ</t>
+  </si>
+  <si>
+    <t>Smart fortwo cabrio electric drive/EQ/Ink Batterie 1Ha</t>
+  </si>
+  <si>
+    <t>Smart ForTwo Coupe electric drive / EQ **COOL&amp;AUDIO**</t>
   </si>
 </sst>
 </file>
@@ -892,7 +958,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC75D6E0-055B-4EAB-9665-2EF495132E7E}">
-  <dimension ref="A1:C1275"/>
+  <dimension ref="A1:C1485"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -14923,6 +14989,2316 @@
         <v>13290</v>
       </c>
     </row>
+    <row r="1276" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A1276" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1276">
+        <v>2018</v>
+      </c>
+      <c r="C1276">
+        <v>10770</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A1277" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1277">
+        <v>2020</v>
+      </c>
+      <c r="C1277">
+        <v>14840</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A1278" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1278">
+        <v>2018</v>
+      </c>
+      <c r="C1278">
+        <v>13450</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A1279" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1279">
+        <v>2018</v>
+      </c>
+      <c r="C1279">
+        <v>11990</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A1280" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1280">
+        <v>2019</v>
+      </c>
+      <c r="C1280">
+        <v>13990</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A1281" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1281">
+        <v>2020</v>
+      </c>
+      <c r="C1281">
+        <v>14490</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A1282" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1282">
+        <v>2020</v>
+      </c>
+      <c r="C1282">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1283" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1283">
+        <v>2017</v>
+      </c>
+      <c r="C1283">
+        <v>11940</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A1284" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1284">
+        <v>2019</v>
+      </c>
+      <c r="C1284">
+        <v>14979</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A1285" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1285">
+        <v>2017</v>
+      </c>
+      <c r="C1285">
+        <v>14900</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A1286" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1286">
+        <v>2019</v>
+      </c>
+      <c r="C1286">
+        <v>14999</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A1287" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1287">
+        <v>2020</v>
+      </c>
+      <c r="C1287">
+        <v>14998</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1288" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1288">
+        <v>2018</v>
+      </c>
+      <c r="C1288">
+        <v>12250</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A1289" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1289">
+        <v>2019</v>
+      </c>
+      <c r="C1289">
+        <v>13980</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A1290" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1290">
+        <v>2019</v>
+      </c>
+      <c r="C1290">
+        <v>13980</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A1291" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1291">
+        <v>2019</v>
+      </c>
+      <c r="C1291">
+        <v>12990</v>
+      </c>
+    </row>
+    <row r="1292" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A1292" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1292">
+        <v>2020</v>
+      </c>
+      <c r="C1292">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1293" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A1293" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1293">
+        <v>2018</v>
+      </c>
+      <c r="C1293">
+        <v>13890</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A1294" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1294">
+        <v>2017</v>
+      </c>
+      <c r="C1294">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1295" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1295">
+        <v>2018</v>
+      </c>
+      <c r="C1295">
+        <v>13200</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A1296" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1296">
+        <v>2020</v>
+      </c>
+      <c r="C1296">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A1297" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1297">
+        <v>2020</v>
+      </c>
+      <c r="C1297">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A1298" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1298">
+        <v>2020</v>
+      </c>
+      <c r="C1298">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A1299" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1299">
+        <v>2020</v>
+      </c>
+      <c r="C1299">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A1300" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1300">
+        <v>2020</v>
+      </c>
+      <c r="C1300">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A1301" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1301">
+        <v>2019</v>
+      </c>
+      <c r="C1301">
+        <v>14490</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A1302" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1302">
+        <v>2019</v>
+      </c>
+      <c r="C1302">
+        <v>13950</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1303" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1303">
+        <v>2017</v>
+      </c>
+      <c r="C1303">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="1304" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A1304" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1304">
+        <v>2019</v>
+      </c>
+      <c r="C1304">
+        <v>13999</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A1305" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1305">
+        <v>2019</v>
+      </c>
+      <c r="C1305">
+        <v>11890</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A1306" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1306">
+        <v>2017</v>
+      </c>
+      <c r="C1306">
+        <v>11979</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A1307" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1307">
+        <v>2017</v>
+      </c>
+      <c r="C1307">
+        <v>11979</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A1308" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1308">
+        <v>2020</v>
+      </c>
+      <c r="C1308">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A1309" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1309">
+        <v>2017</v>
+      </c>
+      <c r="C1309">
+        <v>11500</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A1310" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1310">
+        <v>2019</v>
+      </c>
+      <c r="C1310">
+        <v>13850</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A1311" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1311">
+        <v>2019</v>
+      </c>
+      <c r="C1311">
+        <v>14390</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A1312" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1312">
+        <v>2018</v>
+      </c>
+      <c r="C1312">
+        <v>12550</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A1313" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1313">
+        <v>2017</v>
+      </c>
+      <c r="C1313">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A1314" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1314">
+        <v>2017</v>
+      </c>
+      <c r="C1314">
+        <v>12790</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1315" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1315">
+        <v>2018</v>
+      </c>
+      <c r="C1315">
+        <v>12900</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1316" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1316">
+        <v>2018</v>
+      </c>
+      <c r="C1316">
+        <v>14500</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1317" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1317">
+        <v>2018</v>
+      </c>
+      <c r="C1317">
+        <v>11950</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1318" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1318">
+        <v>2019</v>
+      </c>
+      <c r="C1318">
+        <v>14799</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1319" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1319">
+        <v>2017</v>
+      </c>
+      <c r="C1319">
+        <v>14900</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1320" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1320">
+        <v>2019</v>
+      </c>
+      <c r="C1320">
+        <v>13800</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1321" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1321">
+        <v>2019</v>
+      </c>
+      <c r="C1321">
+        <v>13800</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1322" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1322">
+        <v>2016</v>
+      </c>
+      <c r="C1322">
+        <v>12900</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1323" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1323">
+        <v>2018</v>
+      </c>
+      <c r="C1323">
+        <v>12300</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1324" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1324">
+        <v>2019</v>
+      </c>
+      <c r="C1324">
+        <v>14980</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1325" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1325">
+        <v>2019</v>
+      </c>
+      <c r="C1325">
+        <v>14980</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1326" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1326">
+        <v>2018</v>
+      </c>
+      <c r="C1326">
+        <v>12480</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1327" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1327">
+        <v>2018</v>
+      </c>
+      <c r="C1327">
+        <v>12480</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1328" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1328">
+        <v>2019</v>
+      </c>
+      <c r="C1328">
+        <v>12990</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1329" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1329">
+        <v>2019</v>
+      </c>
+      <c r="C1329">
+        <v>13990</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1330" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1330">
+        <v>2020</v>
+      </c>
+      <c r="C1330">
+        <v>13990</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1331" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1331">
+        <v>2017</v>
+      </c>
+      <c r="C1331">
+        <v>13980</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1332" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1332">
+        <v>2019</v>
+      </c>
+      <c r="C1332">
+        <v>12950</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1333" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1333">
+        <v>2020</v>
+      </c>
+      <c r="C1333">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1334" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1334">
+        <v>2020</v>
+      </c>
+      <c r="C1334">
+        <v>14890</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1335" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1335">
+        <v>2020</v>
+      </c>
+      <c r="C1335">
+        <v>13990</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1336" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1336">
+        <v>2020</v>
+      </c>
+      <c r="C1336">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1337" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1337">
+        <v>2020</v>
+      </c>
+      <c r="C1337">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1338" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1338">
+        <v>2018</v>
+      </c>
+      <c r="C1338">
+        <v>13900</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1339" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1339">
+        <v>2015</v>
+      </c>
+      <c r="C1339">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1340" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1340">
+        <v>2018</v>
+      </c>
+      <c r="C1340">
+        <v>14750</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1341" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1341">
+        <v>2017</v>
+      </c>
+      <c r="C1341">
+        <v>13490</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1342" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1342">
+        <v>2020</v>
+      </c>
+      <c r="C1342">
+        <v>14390</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1343" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1343">
+        <v>2020</v>
+      </c>
+      <c r="C1343">
+        <v>14390</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1344" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1344">
+        <v>2018</v>
+      </c>
+      <c r="C1344">
+        <v>11900</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1345" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1345">
+        <v>2020</v>
+      </c>
+      <c r="C1345">
+        <v>14390</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1346" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1346">
+        <v>2020</v>
+      </c>
+      <c r="C1346">
+        <v>14390</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1347" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1347">
+        <v>2020</v>
+      </c>
+      <c r="C1347">
+        <v>14390</v>
+      </c>
+    </row>
+    <row r="1348" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1348" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1348">
+        <v>2017</v>
+      </c>
+      <c r="C1348">
+        <v>12390</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1349" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1349">
+        <v>2020</v>
+      </c>
+      <c r="C1349">
+        <v>14849</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1350" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1350">
+        <v>2020</v>
+      </c>
+      <c r="C1350">
+        <v>14849</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1351" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1351">
+        <v>2018</v>
+      </c>
+      <c r="C1351">
+        <v>14950</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1352" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1352">
+        <v>2019</v>
+      </c>
+      <c r="C1352">
+        <v>12510</v>
+      </c>
+    </row>
+    <row r="1353" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1353" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1353">
+        <v>2017</v>
+      </c>
+      <c r="C1353">
+        <v>12990</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1354" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1354">
+        <v>2018</v>
+      </c>
+      <c r="C1354">
+        <v>14900</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1355" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1355">
+        <v>2020</v>
+      </c>
+      <c r="C1355">
+        <v>14980</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1356" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1356">
+        <v>2019</v>
+      </c>
+      <c r="C1356">
+        <v>13600</v>
+      </c>
+    </row>
+    <row r="1357" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1357" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1357">
+        <v>2020</v>
+      </c>
+      <c r="C1357">
+        <v>14555</v>
+      </c>
+    </row>
+    <row r="1358" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1358" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1358">
+        <v>2020</v>
+      </c>
+      <c r="C1358">
+        <v>14890</v>
+      </c>
+    </row>
+    <row r="1359" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1359" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1359">
+        <v>2018</v>
+      </c>
+      <c r="C1359">
+        <v>12799</v>
+      </c>
+    </row>
+    <row r="1360" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1360" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1360">
+        <v>2018</v>
+      </c>
+      <c r="C1360">
+        <v>11980</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1361" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1361">
+        <v>2017</v>
+      </c>
+      <c r="C1361">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1362" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1362" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1362">
+        <v>2017</v>
+      </c>
+      <c r="C1362">
+        <v>11855</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1363" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1363">
+        <v>2018</v>
+      </c>
+      <c r="C1363">
+        <v>12888</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1364" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1364">
+        <v>2017</v>
+      </c>
+      <c r="C1364">
+        <v>12890</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1365" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1365">
+        <v>2018</v>
+      </c>
+      <c r="C1365">
+        <v>13888</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1366" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1366">
+        <v>2015</v>
+      </c>
+      <c r="C1366">
+        <v>10900</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1367" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1367">
+        <v>2020</v>
+      </c>
+      <c r="C1367">
+        <v>14890</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1368" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1368">
+        <v>2019</v>
+      </c>
+      <c r="C1368">
+        <v>11950</v>
+      </c>
+    </row>
+    <row r="1369" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1369" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1369">
+        <v>2019</v>
+      </c>
+      <c r="C1369">
+        <v>11950</v>
+      </c>
+    </row>
+    <row r="1370" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1370" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1370">
+        <v>2020</v>
+      </c>
+      <c r="C1370">
+        <v>14890</v>
+      </c>
+    </row>
+    <row r="1371" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1371" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1371">
+        <v>2020</v>
+      </c>
+      <c r="C1371">
+        <v>14890</v>
+      </c>
+    </row>
+    <row r="1372" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1372" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1372">
+        <v>2020</v>
+      </c>
+      <c r="C1372">
+        <v>14290</v>
+      </c>
+    </row>
+    <row r="1373" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1373" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1373">
+        <v>2020</v>
+      </c>
+      <c r="C1373">
+        <v>14290</v>
+      </c>
+    </row>
+    <row r="1374" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1374" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1374">
+        <v>2019</v>
+      </c>
+      <c r="C1374">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1375" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1375" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1375">
+        <v>2018</v>
+      </c>
+      <c r="C1375">
+        <v>11990</v>
+      </c>
+    </row>
+    <row r="1376" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1376" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1376">
+        <v>2018</v>
+      </c>
+      <c r="C1376">
+        <v>13880</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1377" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1377">
+        <v>2019</v>
+      </c>
+      <c r="C1377">
+        <v>13599</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1378" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1378">
+        <v>2018</v>
+      </c>
+      <c r="C1378">
+        <v>13700</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1379" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1379">
+        <v>2018</v>
+      </c>
+      <c r="C1379">
+        <v>13790</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1380" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1380">
+        <v>2017</v>
+      </c>
+      <c r="C1380">
+        <v>12650</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1381" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1381">
+        <v>2018</v>
+      </c>
+      <c r="C1381">
+        <v>14900</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1382" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1382">
+        <v>2018</v>
+      </c>
+      <c r="C1382">
+        <v>12900</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1383" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1383">
+        <v>2019</v>
+      </c>
+      <c r="C1383">
+        <v>14480</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1384" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1384">
+        <v>2020</v>
+      </c>
+      <c r="C1384">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1385" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1385">
+        <v>2020</v>
+      </c>
+      <c r="C1385">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1386" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1386">
+        <v>2020</v>
+      </c>
+      <c r="C1386">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1387" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1387">
+        <v>2020</v>
+      </c>
+      <c r="C1387">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1388" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1388">
+        <v>2020</v>
+      </c>
+      <c r="C1388">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1389" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1389">
+        <v>2020</v>
+      </c>
+      <c r="C1389">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1390" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1390">
+        <v>2020</v>
+      </c>
+      <c r="C1390">
+        <v>14890</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1391" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1391">
+        <v>2020</v>
+      </c>
+      <c r="C1391">
+        <v>14890</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1392" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1392">
+        <v>2020</v>
+      </c>
+      <c r="C1392">
+        <v>14890</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1393" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1393">
+        <v>2020</v>
+      </c>
+      <c r="C1393">
+        <v>14890</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1394" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1394">
+        <v>2020</v>
+      </c>
+      <c r="C1394">
+        <v>14890</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1395" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1395">
+        <v>2019</v>
+      </c>
+      <c r="C1395">
+        <v>13999</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1396" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1396">
+        <v>2019</v>
+      </c>
+      <c r="C1396">
+        <v>14800</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1397" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1397">
+        <v>2019</v>
+      </c>
+      <c r="C1397">
+        <v>14800</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1398" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1398">
+        <v>2017</v>
+      </c>
+      <c r="C1398">
+        <v>14600</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1399" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1399">
+        <v>2021</v>
+      </c>
+      <c r="C1399">
+        <v>14999</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1400" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1400">
+        <v>2020</v>
+      </c>
+      <c r="C1400">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1401" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1401">
+        <v>2018</v>
+      </c>
+      <c r="C1401">
+        <v>14444</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1402" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1402">
+        <v>2017</v>
+      </c>
+      <c r="C1402">
+        <v>13990</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1403" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1403">
+        <v>2019</v>
+      </c>
+      <c r="C1403">
+        <v>14466</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1404" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1404">
+        <v>2019</v>
+      </c>
+      <c r="C1404">
+        <v>13490</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1405" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1405">
+        <v>2019</v>
+      </c>
+      <c r="C1405">
+        <v>13490</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1406" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1406">
+        <v>2019</v>
+      </c>
+      <c r="C1406">
+        <v>13900</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1407" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1407">
+        <v>2020</v>
+      </c>
+      <c r="C1407">
+        <v>12990</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1408" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1408">
+        <v>2019</v>
+      </c>
+      <c r="C1408">
+        <v>13400</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1409" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1409">
+        <v>2020</v>
+      </c>
+      <c r="C1409">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1410" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1410">
+        <v>2018</v>
+      </c>
+      <c r="C1410">
+        <v>13890</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1411" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1411">
+        <v>2018</v>
+      </c>
+      <c r="C1411">
+        <v>12900</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1412" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1412">
+        <v>2018</v>
+      </c>
+      <c r="C1412">
+        <v>14595</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1413" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1413">
+        <v>2019</v>
+      </c>
+      <c r="C1413">
+        <v>14880</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1414" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1414">
+        <v>2018</v>
+      </c>
+      <c r="C1414">
+        <v>13790</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1415" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1415">
+        <v>2020</v>
+      </c>
+      <c r="C1415">
+        <v>13999</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1416" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1416">
+        <v>2018</v>
+      </c>
+      <c r="C1416">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1417" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1417">
+        <v>2017</v>
+      </c>
+      <c r="C1417">
+        <v>13800</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1418" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1418">
+        <v>2020</v>
+      </c>
+      <c r="C1418">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1419" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1419">
+        <v>2017</v>
+      </c>
+      <c r="C1419">
+        <v>13750</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1420" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1420">
+        <v>2017</v>
+      </c>
+      <c r="C1420">
+        <v>11990</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1421" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1421">
+        <v>2018</v>
+      </c>
+      <c r="C1421">
+        <v>12999</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1422" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1422">
+        <v>2018</v>
+      </c>
+      <c r="C1422">
+        <v>12999</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1423" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1423">
+        <v>2018</v>
+      </c>
+      <c r="C1423">
+        <v>12999</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1424" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1424">
+        <v>2018</v>
+      </c>
+      <c r="C1424">
+        <v>12999</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1425" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1425">
+        <v>2018</v>
+      </c>
+      <c r="C1425">
+        <v>12999</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1426" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1426">
+        <v>2018</v>
+      </c>
+      <c r="C1426">
+        <v>14490</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1427" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1427">
+        <v>2017</v>
+      </c>
+      <c r="C1427">
+        <v>13990</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1428" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1428">
+        <v>2018</v>
+      </c>
+      <c r="C1428">
+        <v>13250</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1429" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1429">
+        <v>2019</v>
+      </c>
+      <c r="C1429">
+        <v>14990</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1430" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1430">
+        <v>2017</v>
+      </c>
+      <c r="C1430">
+        <v>14290</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1431" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1431">
+        <v>2017</v>
+      </c>
+      <c r="C1431">
+        <v>13390</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1432" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1432">
+        <v>2019</v>
+      </c>
+      <c r="C1432">
+        <v>12950</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1433" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1433">
+        <v>2017</v>
+      </c>
+      <c r="C1433">
+        <v>12690</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1434" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1434">
+        <v>2018</v>
+      </c>
+      <c r="C1434">
+        <v>11990</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1435" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1435">
+        <v>2019</v>
+      </c>
+      <c r="C1435">
+        <v>13990</v>
+      </c>
+    </row>
+    <row r="1436" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1436" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1436">
+        <v>2018</v>
+      </c>
+      <c r="C1436">
+        <v>11720</v>
+      </c>
+    </row>
+    <row r="1437" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1437" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1437">
+        <v>2017</v>
+      </c>
+      <c r="C1437">
+        <v>13333</v>
+      </c>
+    </row>
+    <row r="1438" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1438" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1438">
+        <v>2013</v>
+      </c>
+      <c r="C1438">
+        <v>10400</v>
+      </c>
+    </row>
+    <row r="1439" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1439" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1439">
+        <v>2018</v>
+      </c>
+      <c r="C1439">
+        <v>13250</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1440" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1440">
+        <v>2018</v>
+      </c>
+      <c r="C1440">
+        <v>12990</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1441" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1441">
+        <v>2018</v>
+      </c>
+      <c r="C1441">
+        <v>12990</v>
+      </c>
+    </row>
+    <row r="1442" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1442" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1442">
+        <v>2019</v>
+      </c>
+      <c r="C1442">
+        <v>13900</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1443" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1443">
+        <v>2019</v>
+      </c>
+      <c r="C1443">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1444" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1444">
+        <v>2019</v>
+      </c>
+      <c r="C1444">
+        <v>13930</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1445" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1445">
+        <v>2018</v>
+      </c>
+      <c r="C1445">
+        <v>12689</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1446" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1446">
+        <v>2020</v>
+      </c>
+      <c r="C1446">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1447" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1447">
+        <v>2018</v>
+      </c>
+      <c r="C1447">
+        <v>12689</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1448" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1448">
+        <v>2018</v>
+      </c>
+      <c r="C1448">
+        <v>12689</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1449" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1449">
+        <v>2018</v>
+      </c>
+      <c r="C1449">
+        <v>13990</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1450" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1450">
+        <v>2014</v>
+      </c>
+      <c r="C1450">
+        <v>13479</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1451" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1451">
+        <v>2018</v>
+      </c>
+      <c r="C1451">
+        <v>12195</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1452" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1452">
+        <v>2018</v>
+      </c>
+      <c r="C1452">
+        <v>10490</v>
+      </c>
+    </row>
+    <row r="1453" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1453" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1453">
+        <v>2019</v>
+      </c>
+      <c r="C1453">
+        <v>14979</v>
+      </c>
+    </row>
+    <row r="1454" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1454" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1454">
+        <v>2018</v>
+      </c>
+      <c r="C1454">
+        <v>11290</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1455" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1455">
+        <v>2018</v>
+      </c>
+      <c r="C1455">
+        <v>12490</v>
+      </c>
+    </row>
+    <row r="1456" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1456" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1456">
+        <v>2018</v>
+      </c>
+      <c r="C1456">
+        <v>14490</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1457" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1457">
+        <v>2018</v>
+      </c>
+      <c r="C1457">
+        <v>14490</v>
+      </c>
+    </row>
+    <row r="1458" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1458" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1458">
+        <v>2019</v>
+      </c>
+      <c r="C1458">
+        <v>12900</v>
+      </c>
+    </row>
+    <row r="1459" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1459" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1459">
+        <v>2019</v>
+      </c>
+      <c r="C1459">
+        <v>14900</v>
+      </c>
+    </row>
+    <row r="1460" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1460" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1460">
+        <v>2018</v>
+      </c>
+      <c r="C1460">
+        <v>12099</v>
+      </c>
+    </row>
+    <row r="1461" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1461" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1461">
+        <v>2018</v>
+      </c>
+      <c r="C1461">
+        <v>12499</v>
+      </c>
+    </row>
+    <row r="1462" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1462" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1462">
+        <v>2020</v>
+      </c>
+      <c r="C1462">
+        <v>14875</v>
+      </c>
+    </row>
+    <row r="1463" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1463" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1463">
+        <v>2018</v>
+      </c>
+      <c r="C1463">
+        <v>12966</v>
+      </c>
+    </row>
+    <row r="1464" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1464" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1464">
+        <v>2019</v>
+      </c>
+      <c r="C1464">
+        <v>12820</v>
+      </c>
+    </row>
+    <row r="1465" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1465" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1465">
+        <v>2018</v>
+      </c>
+      <c r="C1465">
+        <v>12900</v>
+      </c>
+    </row>
+    <row r="1466" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1466" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1466">
+        <v>2018</v>
+      </c>
+      <c r="C1466">
+        <v>12900</v>
+      </c>
+    </row>
+    <row r="1467" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1467" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1467">
+        <v>2018</v>
+      </c>
+      <c r="C1467">
+        <v>12900</v>
+      </c>
+    </row>
+    <row r="1468" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1468" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1468">
+        <v>2014</v>
+      </c>
+      <c r="C1468">
+        <v>11111</v>
+      </c>
+    </row>
+    <row r="1469" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1469" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1469">
+        <v>2017</v>
+      </c>
+      <c r="C1469">
+        <v>12450</v>
+      </c>
+    </row>
+    <row r="1470" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1470" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1470">
+        <v>2014</v>
+      </c>
+      <c r="C1470">
+        <v>13200</v>
+      </c>
+    </row>
+    <row r="1471" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1471" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1471">
+        <v>2018</v>
+      </c>
+      <c r="C1471">
+        <v>11990</v>
+      </c>
+    </row>
+    <row r="1472" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1472" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1472">
+        <v>2018</v>
+      </c>
+      <c r="C1472">
+        <v>11990</v>
+      </c>
+    </row>
+    <row r="1473" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1473" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1473">
+        <v>2017</v>
+      </c>
+      <c r="C1473">
+        <v>13980</v>
+      </c>
+    </row>
+    <row r="1474" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1474" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1474">
+        <v>2017</v>
+      </c>
+      <c r="C1474">
+        <v>12490</v>
+      </c>
+    </row>
+    <row r="1475" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1475" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1475">
+        <v>2018</v>
+      </c>
+      <c r="C1475">
+        <v>12985</v>
+      </c>
+    </row>
+    <row r="1476" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1476" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1476">
+        <v>2018</v>
+      </c>
+      <c r="C1476">
+        <v>12985</v>
+      </c>
+    </row>
+    <row r="1477" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1477" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1477">
+        <v>2017</v>
+      </c>
+      <c r="C1477">
+        <v>14995</v>
+      </c>
+    </row>
+    <row r="1478" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1478" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1478">
+        <v>2018</v>
+      </c>
+      <c r="C1478">
+        <v>11600</v>
+      </c>
+    </row>
+    <row r="1479" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1479" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1479">
+        <v>2018</v>
+      </c>
+      <c r="C1479">
+        <v>12490</v>
+      </c>
+    </row>
+    <row r="1480" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1480" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1480">
+        <v>2018</v>
+      </c>
+      <c r="C1480">
+        <v>12490</v>
+      </c>
+    </row>
+    <row r="1481" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1481" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1481">
+        <v>2017</v>
+      </c>
+      <c r="C1481">
+        <v>11450</v>
+      </c>
+    </row>
+    <row r="1482" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1482" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1482">
+        <v>2018</v>
+      </c>
+      <c r="C1482">
+        <v>11999</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1483" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1483">
+        <v>2014</v>
+      </c>
+      <c r="C1483">
+        <v>13490</v>
+      </c>
+    </row>
+    <row r="1484" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1484" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1484">
+        <v>2017</v>
+      </c>
+      <c r="C1484">
+        <v>13290</v>
+      </c>
+    </row>
+    <row r="1485" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1485" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1485">
+        <v>2017</v>
+      </c>
+      <c r="C1485">
+        <v>13290</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>